<commit_message>
Add another sheet for range cursor in split sheet view.
</commit_message>
<xml_diff>
--- a/test/xlsx/view/cursor-split-pane.xlsx
+++ b/test/xlsx/view/cursor-split-pane.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,19 +9,38 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19680" windowHeight="8760" tabRatio="841"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19680" windowHeight="8760" tabRatio="841" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>cursor</t>
+  </si>
+  <si>
+    <t>top-left</t>
+  </si>
+  <si>
+    <t>bottom-right</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>bottom</t>
   </si>
 </sst>
 </file>
@@ -870,7 +889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5190" ySplit="1800" topLeftCell="F6" activePane="bottomLeft"/>
       <selection activeCell="E4" sqref="E4"/>
       <selection pane="topRight" activeCell="J2" sqref="J2"/>
@@ -903,4 +922,98 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:L23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5190" ySplit="2400" topLeftCell="F8" activePane="topRight"/>
+      <selection activeCell="C2" sqref="C2:C6"/>
+      <selection pane="topRight" activeCell="H2" sqref="H2:L2"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18:C23"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11:J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="H11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
xlsx: add two more sheets.
</commit_message>
<xml_diff>
--- a/test/xlsx/view/cursor-split-pane.xlsx
+++ b/test/xlsx/view/cursor-split-pane.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,18 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19680" windowHeight="8760" tabRatio="841" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19680" windowHeight="8760" tabRatio="841" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
   <si>
     <t>cursor</t>
   </si>
@@ -928,7 +930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5190" ySplit="2400" topLeftCell="F8" activePane="topRight"/>
       <selection activeCell="C2" sqref="C2:C6"/>
       <selection pane="topRight" activeCell="H2" sqref="H2:L2"/>
@@ -1016,4 +1018,58 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1500" topLeftCell="A5" activePane="bottomLeft"/>
+      <selection activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B11:I18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4230" topLeftCell="E1"/>
+      <selection activeCell="B18" sqref="B18"/>
+      <selection pane="topRight" activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="11" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>